<commit_message>
first steps with software
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\RCK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29CA386-66C8-452C-87D9-0DDF61B1C093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DF3CC0-77FE-49FB-9082-D2E95161869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="5160" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{E375E285-8F85-42C4-8603-06EDA8FA43E9}"/>
   </bookViews>
@@ -929,6 +929,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -966,69 +1029,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1354,7 +1354,7 @@
   <dimension ref="C1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,16 +1372,16 @@
   <sheetData>
     <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1411,10 +1411,10 @@
       </c>
     </row>
     <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="62" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="36" t="s">
@@ -1426,19 +1426,19 @@
       <c r="G5" s="36">
         <v>16</v>
       </c>
-      <c r="H5" s="58">
+      <c r="H5" s="45">
         <v>3.78</v>
       </c>
-      <c r="I5" s="58">
+      <c r="I5" s="45">
         <v>0.73</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="48" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="74"/>
-      <c r="D6" s="76"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="8" t="s">
         <v>33</v>
       </c>
@@ -1448,13 +1448,13 @@
       <c r="G6" s="8">
         <v>16</v>
       </c>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="62"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="49"/>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="74"/>
-      <c r="D7" s="76"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="63"/>
       <c r="E7" s="8" t="s">
         <v>31</v>
       </c>
@@ -1464,13 +1464,13 @@
       <c r="G7" s="8">
         <v>16</v>
       </c>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="62"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="49"/>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="74"/>
-      <c r="D8" s="76"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="63"/>
       <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
@@ -1480,15 +1480,15 @@
       <c r="G8" s="8">
         <v>16</v>
       </c>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="63"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="50"/>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="78" t="s">
+      <c r="D9" s="65" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1500,20 +1500,20 @@
       <c r="G9" s="5">
         <v>20</v>
       </c>
-      <c r="H9" s="64">
+      <c r="H9" s="51">
         <v>3.49</v>
       </c>
-      <c r="I9" s="64">
+      <c r="I9" s="51">
         <v>0</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="54" t="s">
         <v>42</v>
       </c>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="77"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
       <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
@@ -1523,13 +1523,13 @@
       <c r="G10" s="5">
         <v>20</v>
       </c>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="68"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="77"/>
-      <c r="D11" s="78"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="65"/>
       <c r="E11" s="5" t="s">
         <v>35</v>
       </c>
@@ -1539,9 +1539,9 @@
       <c r="G11" s="5">
         <v>20</v>
       </c>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="69"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="9" t="s">
@@ -1586,7 +1586,7 @@
         <v>100</v>
       </c>
       <c r="H13" s="27">
-        <v>13.26</v>
+        <v>13.28</v>
       </c>
       <c r="I13" s="33">
         <v>0</v>
@@ -1804,10 +1804,10 @@
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D22" s="74" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -1819,19 +1819,19 @@
       <c r="G22" s="8">
         <v>4</v>
       </c>
-      <c r="H22" s="55">
-        <v>18.809999999999999</v>
-      </c>
-      <c r="I22" s="55">
+      <c r="H22" s="76">
+        <v>12.55</v>
+      </c>
+      <c r="I22" s="76">
         <v>0</v>
       </c>
-      <c r="J22" s="56" t="s">
+      <c r="J22" s="77" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="52"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="28" t="s">
         <v>65</v>
       </c>
@@ -1841,12 +1841,12 @@
       <c r="G23" s="8">
         <v>1</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="57"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="76"/>
+      <c r="J23" s="78"/>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="68" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="18" t="s">
@@ -1867,12 +1867,12 @@
       <c r="I24" s="41">
         <v>0</v>
       </c>
-      <c r="J24" s="49" t="s">
+      <c r="J24" s="70" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="48"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="18" t="s">
         <v>71</v>
       </c>
@@ -1885,13 +1885,9 @@
       <c r="G25" s="19">
         <v>5</v>
       </c>
-      <c r="H25" s="41">
-        <v>45.1</v>
-      </c>
-      <c r="I25" s="41">
-        <v>0</v>
-      </c>
-      <c r="J25" s="50"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="71"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
@@ -1952,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="42">
-        <v>8.4600000000000009</v>
+        <v>12.22</v>
       </c>
       <c r="I29" s="43">
         <v>0</v>
@@ -1968,7 +1964,7 @@
       </c>
       <c r="H31" s="3">
         <f>SUM(H5:H29)</f>
-        <v>147.4</v>
+        <v>99.82</v>
       </c>
       <c r="I31" s="38">
         <f>SUM(I5:I29)</f>
@@ -1976,14 +1972,22 @@
       </c>
     </row>
     <row r="32" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H32" s="45">
+      <c r="H32" s="66">
         <f>SUM(H31:I31)</f>
-        <v>153.28</v>
-      </c>
-      <c r="I32" s="46"/>
+        <v>105.69999999999999</v>
+      </c>
+      <c r="I32" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
     <mergeCell ref="H5:H8"/>
     <mergeCell ref="J5:J8"/>
     <mergeCell ref="H9:H11"/>
@@ -1995,14 +1999,6 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="I5:I8"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" xr:uid="{1AEBCBEE-4BEB-4EAB-A7FB-C675A1B10379}"/>

</xml_diff>